<commit_message>
fix headRow, update doc
</commit_message>
<xml_diff>
--- a/example/i18n/langs/_todo_en.xlsx
+++ b/example/i18n/langs/_todo_en.xlsx
@@ -565,7 +565,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>杀个怪</t>
+          <t>和npc对话</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>杀怪</t>
+          <t>和npc对话</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>和npc对话</t>
+          <t>收集物品</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>和npc对话</t>
+          <t>收集物品</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>收集物品</t>
+          <t>杀怪并且收集物品</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>收集物品</t>
+          <t>杀怪并且收集物品</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>杀怪并且收集物品</t>
+          <t>杀怪对话并且收集物品</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>杀怪并且收集物品</t>
+          <t>杀怪对话并且收集物品</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>杀怪对话并且收集物品</t>
+          <t>聊天并且杀怪</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>杀怪对话并且收集物品</t>
+          <t>测试转义符号</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -845,7 +845,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>聊天并且杀怪</t>
+          <t>测试</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>测试转义符号</t>
+          <t>测试无参数得bean</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>测试</t>
+          <t>测试2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>测试无参数得bean</t>
+          <t>测试默认bean</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -938,12 +938,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>task.task</t>
+          <t>task.task2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>测试2</t>
+          <t>测试用</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -965,22 +965,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>task.task</t>
+          <t>task.task2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>name-1</t>
+          <t>name-0</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>测试默认bean</t>
+          <t>和npc对话</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -997,17 +997,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>name-0</t>
+          <t>name-1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>测试用</t>
+          <t>和npc对话</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>和npc对话</t>
+          <t>收集物品</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>和npc对话</t>
+          <t>收集物品</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>收集物品</t>
+          <t>杀怪并且收集物品</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>收集物品</t>
+          <t>杀怪并且收集物品</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>杀怪并且收集物品</t>
+          <t>杀怪对话并且收集物品</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>杀怪并且收集物品</t>
+          <t>杀怪对话并且收集物品</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>杀怪对话并且收集物品</t>
+          <t>聊天并且杀怪</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>杀怪对话并且收集物品</t>
+          <t>测试转义符号</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>聊天并且杀怪</t>
+          <t>测试</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>测试转义符号</t>
+          <t>测试无参数得bean</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>测试</t>
+          <t>测试2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1331,64 +1331,10 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>测试无参数得bean</t>
+          <t>测试默认bean</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>task.task2</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>name-0</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>测试2</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>task.task2</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>name-1</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>测试默认bean</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1418,7 +1364,7 @@
     <col min="1" max="1" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1526,6 +1472,60 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>abc</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>task.task</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>name-0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>杀个怪</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>kill a monster</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>task.task</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>name-1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>杀怪</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>kill monster</t>
         </is>
       </c>
     </row>

</xml_diff>